<commit_message>
Completed interim report for submission
</commit_message>
<xml_diff>
--- a/Docs/InterimReport/Gantt Chart.xlsx
+++ b/Docs/InterimReport/Gantt Chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitRepos\Uni\Thesis\Docs\InterimReport\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DB19AE5-7544-43D3-AAC2-F912874F27DA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51FEE479-8F23-4A53-A631-DA00BEAB9ABE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -565,9 +565,6 @@
     <t>Time dilation research and prototype</t>
   </si>
   <si>
-    <t>COMPUTER VISION</t>
-  </si>
-  <si>
     <t>Python vs C++ research</t>
   </si>
   <si>
@@ -662,6 +659,9 @@
   </si>
   <si>
     <t>AS AT 24 MAY 19</t>
+  </si>
+  <si>
+    <t>COMPUTER VISION BASICS</t>
   </si>
 </sst>
 </file>
@@ -1101,6 +1101,12 @@
     <xf numFmtId="0" fontId="11" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1108,12 +1114,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1596,8 +1596,8 @@
   <dimension ref="A1:IQ61"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="70" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AF12" sqref="AF12"/>
+      <pane ySplit="3" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D52" sqref="D52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1616,8 +1616,8 @@
       <c r="A1" s="21" t="s">
         <v>165</v>
       </c>
-      <c r="B1" s="32" t="s">
-        <v>206</v>
+      <c r="B1" s="28" t="s">
+        <v>205</v>
       </c>
       <c r="F1" s="7" t="s">
         <v>1</v>
@@ -1626,67 +1626,67 @@
         <v>13</v>
       </c>
       <c r="I1" s="9"/>
-      <c r="J1" s="28" t="s">
+      <c r="J1" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="29"/>
-      <c r="L1" s="29"/>
-      <c r="M1" s="29"/>
-      <c r="N1" s="30"/>
+      <c r="K1" s="31"/>
+      <c r="L1" s="31"/>
+      <c r="M1" s="31"/>
+      <c r="N1" s="32"/>
       <c r="O1" s="10"/>
-      <c r="P1" s="28" t="s">
+      <c r="P1" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="Q1" s="29"/>
-      <c r="R1" s="29"/>
-      <c r="S1" s="30"/>
+      <c r="Q1" s="31"/>
+      <c r="R1" s="31"/>
+      <c r="S1" s="32"/>
       <c r="T1" s="11"/>
-      <c r="U1" s="28" t="s">
+      <c r="U1" s="30" t="s">
         <v>160</v>
       </c>
-      <c r="V1" s="29"/>
-      <c r="W1" s="29"/>
-      <c r="X1" s="30"/>
+      <c r="V1" s="31"/>
+      <c r="W1" s="31"/>
+      <c r="X1" s="32"/>
       <c r="Y1" s="12"/>
-      <c r="Z1" s="28" t="s">
+      <c r="Z1" s="30" t="s">
         <v>161</v>
       </c>
-      <c r="AA1" s="29"/>
-      <c r="AB1" s="29"/>
-      <c r="AC1" s="29"/>
-      <c r="AD1" s="29"/>
-      <c r="AE1" s="29"/>
-      <c r="AF1" s="30"/>
+      <c r="AA1" s="31"/>
+      <c r="AB1" s="31"/>
+      <c r="AC1" s="31"/>
+      <c r="AD1" s="31"/>
+      <c r="AE1" s="31"/>
+      <c r="AF1" s="32"/>
       <c r="AG1" s="13"/>
-      <c r="AH1" s="28" t="s">
+      <c r="AH1" s="30" t="s">
         <v>162</v>
       </c>
-      <c r="AI1" s="29"/>
-      <c r="AJ1" s="29"/>
-      <c r="AK1" s="29"/>
-      <c r="AL1" s="29"/>
-      <c r="AM1" s="29"/>
-      <c r="AN1" s="29"/>
-      <c r="AO1" s="29"/>
+      <c r="AI1" s="31"/>
+      <c r="AJ1" s="31"/>
+      <c r="AK1" s="31"/>
+      <c r="AL1" s="31"/>
+      <c r="AM1" s="31"/>
+      <c r="AN1" s="31"/>
+      <c r="AO1" s="31"/>
       <c r="AQ1" s="24"/>
     </row>
     <row r="2" spans="1:251" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="31" t="s">
+      <c r="B2" s="29" t="s">
         <v>158</v>
       </c>
-      <c r="C2" s="31" t="s">
+      <c r="C2" s="29" t="s">
         <v>159</v>
       </c>
-      <c r="D2" s="31" t="s">
+      <c r="D2" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="31" t="s">
+      <c r="E2" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="31" t="s">
+      <c r="F2" s="29" t="s">
         <v>4</v>
       </c>
       <c r="G2" s="14">
@@ -2426,12 +2426,12 @@
       </c>
     </row>
     <row r="3" spans="1:251" s="1" customFormat="1" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="31"/>
-      <c r="B3" s="31"/>
-      <c r="C3" s="31"/>
-      <c r="D3" s="31"/>
-      <c r="E3" s="31"/>
-      <c r="F3" s="31"/>
+      <c r="A3" s="29"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
       <c r="G3" s="16">
         <v>43521</v>
       </c>
@@ -3263,7 +3263,7 @@
     </row>
     <row r="4" spans="1:251" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="22" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B4" s="22">
         <f>MIN(B5:B9)</f>
@@ -3282,7 +3282,7 @@
         <v>12</v>
       </c>
       <c r="F4" s="23">
-        <f>(F5*C5+F6*C6+F7*C7+F8*C8+F9*C9)/SUM(C5:C8)</f>
+        <f>(F5*C5+F6*C6+F7*C7+F8*C8+F9*C9)/SUM(C5:C9)</f>
         <v>1</v>
       </c>
       <c r="G4" s="15"/>
@@ -4608,7 +4608,7 @@
         <v>3</v>
       </c>
       <c r="F9" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G9" s="15"/>
       <c r="H9" s="15"/>
@@ -6178,7 +6178,7 @@
     </row>
     <row r="15" spans="1:251" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B15" s="3">
         <v>13</v>
@@ -6443,13 +6443,16 @@
     </row>
     <row r="16" spans="1:251" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B16" s="3">
         <v>14</v>
       </c>
       <c r="C16" s="1">
         <v>1</v>
+      </c>
+      <c r="F16" s="5">
+        <v>0</v>
       </c>
       <c r="G16" s="15"/>
       <c r="H16" s="15"/>
@@ -6699,13 +6702,16 @@
     </row>
     <row r="17" spans="1:251" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B17" s="3">
         <v>14</v>
       </c>
       <c r="C17" s="1">
         <v>6</v>
+      </c>
+      <c r="F17" s="5">
+        <v>0</v>
       </c>
       <c r="G17" s="15"/>
       <c r="H17" s="15"/>
@@ -6955,13 +6961,16 @@
     </row>
     <row r="18" spans="1:251" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B18" s="3">
         <v>26</v>
       </c>
       <c r="C18" s="1">
         <v>2</v>
+      </c>
+      <c r="F18" s="5">
+        <v>0</v>
       </c>
       <c r="G18" s="15"/>
       <c r="H18" s="15"/>
@@ -7463,7 +7472,7 @@
     </row>
     <row r="20" spans="1:251" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="22" t="s">
-        <v>174</v>
+        <v>206</v>
       </c>
       <c r="B20" s="22">
         <f>MIN(B21:B25)</f>
@@ -7483,7 +7492,7 @@
       </c>
       <c r="F20" s="23">
         <f>(F21*C21+F22*C22+F23*C23+F24*C24+F25*C25)/SUM(C21:C25)</f>
-        <v>0.58333333333333337</v>
+        <v>1</v>
       </c>
       <c r="G20" s="15"/>
       <c r="H20" s="15"/>
@@ -7733,7 +7742,7 @@
     </row>
     <row r="21" spans="1:251" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B21" s="1">
         <v>3</v>
@@ -7998,7 +8007,7 @@
     </row>
     <row r="22" spans="1:251" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B22" s="1">
         <v>3</v>
@@ -8263,7 +8272,7 @@
     </row>
     <row r="23" spans="1:251" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B23" s="1">
         <v>5</v>
@@ -8528,7 +8537,7 @@
     </row>
     <row r="24" spans="1:251" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B24" s="3">
         <v>4</v>
@@ -8543,7 +8552,7 @@
         <v>3</v>
       </c>
       <c r="F24" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G24" s="15"/>
       <c r="H24" s="15"/>
@@ -8793,7 +8802,7 @@
     </row>
     <row r="25" spans="1:251" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B25" s="3">
         <v>7</v>
@@ -8808,7 +8817,7 @@
         <v>3</v>
       </c>
       <c r="F25" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G25" s="15"/>
       <c r="H25" s="15"/>
@@ -9307,7 +9316,7 @@
     </row>
     <row r="27" spans="1:251" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="22" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B27" s="22">
         <f>MIN(B28:B32)</f>
@@ -9577,7 +9586,7 @@
     </row>
     <row r="28" spans="1:251" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B28" s="3">
         <v>7</v>
@@ -9842,7 +9851,7 @@
     </row>
     <row r="29" spans="1:251" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B29" s="3">
         <v>9</v>
@@ -10107,7 +10116,7 @@
     </row>
     <row r="30" spans="1:251" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B30" s="3">
         <v>11</v>
@@ -10372,7 +10381,7 @@
     </row>
     <row r="31" spans="1:251" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B31" s="3">
         <v>14</v>
@@ -10631,7 +10640,7 @@
     </row>
     <row r="32" spans="1:251" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B32" s="3">
         <v>16</v>
@@ -10891,9 +10900,6 @@
     <row r="33" spans="1:251" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
       <c r="B33" s="3"/>
-      <c r="F33" s="5">
-        <v>0</v>
-      </c>
       <c r="G33" s="15"/>
       <c r="H33" s="15"/>
       <c r="I33" s="15"/>
@@ -11142,7 +11148,7 @@
     </row>
     <row r="34" spans="1:251" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="22" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B34" s="22">
         <f>MIN(B35:B39)</f>
@@ -11412,7 +11418,7 @@
     </row>
     <row r="35" spans="1:251" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B35" s="1">
         <v>3</v>
@@ -11677,7 +11683,7 @@
     </row>
     <row r="36" spans="1:251" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B36" s="1">
         <v>10</v>
@@ -11942,7 +11948,7 @@
     </row>
     <row r="37" spans="1:251" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B37" s="1">
         <v>15</v>
@@ -12201,7 +12207,7 @@
     </row>
     <row r="38" spans="1:251" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B38" s="1">
         <v>20</v>
@@ -12460,7 +12466,7 @@
     </row>
     <row r="39" spans="1:251" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B39" s="1">
         <v>24</v>
@@ -12719,13 +12725,16 @@
     </row>
     <row r="40" spans="1:251" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B40" s="1">
         <v>26</v>
       </c>
       <c r="C40" s="1">
         <v>4</v>
+      </c>
+      <c r="F40" s="5">
+        <v>0</v>
       </c>
       <c r="G40" s="15"/>
       <c r="H40" s="15"/>
@@ -12975,13 +12984,16 @@
     </row>
     <row r="41" spans="1:251" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B41" s="1">
         <v>30</v>
       </c>
       <c r="C41" s="1">
         <v>2</v>
+      </c>
+      <c r="F41" s="5">
+        <v>0</v>
       </c>
       <c r="G41" s="15"/>
       <c r="H41" s="15"/>
@@ -13231,9 +13243,6 @@
     </row>
     <row r="42" spans="1:251" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="2"/>
-      <c r="F42" s="5">
-        <v>0</v>
-      </c>
       <c r="G42" s="15"/>
       <c r="H42" s="15"/>
       <c r="I42" s="15"/>
@@ -13482,7 +13491,7 @@
     </row>
     <row r="43" spans="1:251" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="22" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B43" s="22">
         <f>MIN(B44:B48)</f>
@@ -13752,7 +13761,7 @@
     </row>
     <row r="44" spans="1:251" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B44" s="1">
         <v>11</v>
@@ -14017,7 +14026,7 @@
     </row>
     <row r="45" spans="1:251" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B45" s="1">
         <v>12</v>
@@ -14282,7 +14291,7 @@
     </row>
     <row r="46" spans="1:251" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B46" s="1">
         <v>32</v>
@@ -14541,7 +14550,7 @@
     </row>
     <row r="47" spans="1:251" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B47" s="1">
         <v>32</v>
@@ -14800,7 +14809,7 @@
     </row>
     <row r="48" spans="1:251" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B48" s="1">
         <v>34</v>
@@ -15059,7 +15068,7 @@
     </row>
     <row r="49" spans="1:251" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B49" s="1">
         <v>30</v>
@@ -15318,9 +15327,6 @@
     </row>
     <row r="50" spans="1:251" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="2"/>
-      <c r="F50" s="5">
-        <v>0</v>
-      </c>
       <c r="G50" s="15"/>
       <c r="H50" s="15"/>
       <c r="I50" s="15"/>
@@ -15569,9 +15575,6 @@
     </row>
     <row r="51" spans="1:251" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="2"/>
-      <c r="F51" s="5">
-        <v>0</v>
-      </c>
       <c r="G51" s="15"/>
       <c r="H51" s="15"/>
       <c r="I51" s="15"/>
@@ -15820,9 +15823,6 @@
     </row>
     <row r="52" spans="1:251" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="2"/>
-      <c r="F52" s="5">
-        <v>0</v>
-      </c>
       <c r="G52" s="15"/>
       <c r="H52" s="15"/>
       <c r="I52" s="15"/>
@@ -16071,9 +16071,6 @@
     </row>
     <row r="53" spans="1:251" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="2"/>
-      <c r="F53" s="5">
-        <v>0</v>
-      </c>
       <c r="G53" s="15"/>
       <c r="H53" s="15"/>
       <c r="I53" s="15"/>
@@ -16322,9 +16319,6 @@
     </row>
     <row r="54" spans="1:251" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="2"/>
-      <c r="F54" s="5">
-        <v>0</v>
-      </c>
       <c r="G54" s="15"/>
       <c r="H54" s="15"/>
       <c r="I54" s="15"/>
@@ -16573,9 +16567,6 @@
     </row>
     <row r="55" spans="1:251" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="2"/>
-      <c r="F55" s="5">
-        <v>0</v>
-      </c>
       <c r="G55" s="15"/>
       <c r="H55" s="15"/>
       <c r="I55" s="15"/>
@@ -16824,9 +16815,6 @@
     </row>
     <row r="56" spans="1:251" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="2"/>
-      <c r="F56" s="5">
-        <v>0</v>
-      </c>
       <c r="G56" s="15"/>
       <c r="H56" s="15"/>
       <c r="I56" s="15"/>
@@ -17075,9 +17063,6 @@
     </row>
     <row r="57" spans="1:251" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="2"/>
-      <c r="F57" s="5">
-        <v>0</v>
-      </c>
       <c r="G57" s="15"/>
       <c r="H57" s="15"/>
       <c r="I57" s="15"/>
@@ -17326,9 +17311,6 @@
     </row>
     <row r="58" spans="1:251" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="2"/>
-      <c r="F58" s="5">
-        <v>0</v>
-      </c>
       <c r="G58" s="15"/>
       <c r="H58" s="15"/>
       <c r="I58" s="15"/>
@@ -17578,9 +17560,6 @@
     <row r="59" spans="1:251" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="2"/>
       <c r="B59" s="3"/>
-      <c r="F59" s="5">
-        <v>0</v>
-      </c>
       <c r="G59" s="15"/>
       <c r="H59" s="15"/>
       <c r="I59" s="15"/>
@@ -17829,9 +17808,6 @@
     </row>
     <row r="60" spans="1:251" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="2"/>
-      <c r="F60" s="5">
-        <v>0</v>
-      </c>
       <c r="G60" s="15"/>
       <c r="H60" s="15"/>
       <c r="I60" s="15"/>
@@ -18080,9 +18056,6 @@
     </row>
     <row r="61" spans="1:251" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="2"/>
-      <c r="F61" s="5">
-        <v>0</v>
-      </c>
       <c r="G61" s="15"/>
       <c r="H61" s="15"/>
       <c r="I61" s="15"/>
@@ -18331,17 +18304,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="AH1:AO1"/>
+    <mergeCell ref="J1:N1"/>
+    <mergeCell ref="P1:S1"/>
+    <mergeCell ref="U1:X1"/>
+    <mergeCell ref="Z1:AF1"/>
     <mergeCell ref="F2:F3"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="C2:C3"/>
     <mergeCell ref="D2:D3"/>
     <mergeCell ref="E2:E3"/>
-    <mergeCell ref="AH1:AO1"/>
-    <mergeCell ref="J1:N1"/>
-    <mergeCell ref="P1:S1"/>
-    <mergeCell ref="U1:X1"/>
-    <mergeCell ref="Z1:AF1"/>
   </mergeCells>
   <conditionalFormatting sqref="G4:IQ61">
     <cfRule type="expression" dxfId="17" priority="212">

</xml_diff>

<commit_message>
Created test track and waypoint nodes
Updated Gantt chart
Added textures
Created simple terrain with texture based track
Created initial waypoint node setup
</commit_message>
<xml_diff>
--- a/Docs/InterimReport/Gantt Chart.xlsx
+++ b/Docs/InterimReport/Gantt Chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitRepos\Uni\Thesis\Docs\InterimReport\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F1668D7-93D1-4A2A-9757-9DAD3BAACBC7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DBAA3BA-9300-4CAF-87DC-6BC150E07B42}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -658,10 +658,10 @@
     <t>Consolodation of output visualisation products</t>
   </si>
   <si>
-    <t>AS AT 24 MAY 19</t>
-  </si>
-  <si>
     <t>COMPUTER VISION BASICS</t>
+  </si>
+  <si>
+    <t>AS AT 30 MAY 19</t>
   </si>
 </sst>
 </file>
@@ -1596,8 +1596,8 @@
   <dimension ref="A1:IQ61"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="70" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D46" sqref="D46"/>
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AP49" sqref="A1:AP49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1617,7 +1617,7 @@
         <v>165</v>
       </c>
       <c r="B1" s="28" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="F1" s="7" t="s">
         <v>1</v>
@@ -5127,7 +5127,7 @@
       </c>
       <c r="E11" s="22">
         <f>SUM(E12:E19)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F11" s="23">
         <f>(F12*C12+F13*C13+F14*C14)/SUM(C12:C14)</f>
@@ -6452,10 +6452,13 @@
         <v>1</v>
       </c>
       <c r="D16" s="1">
-        <v>15</v>
+        <v>14</v>
+      </c>
+      <c r="E16" s="1">
+        <v>1</v>
       </c>
       <c r="F16" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G16" s="15"/>
       <c r="H16" s="15"/>
@@ -6714,7 +6717,7 @@
         <v>6</v>
       </c>
       <c r="D17" s="1">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F17" s="5">
         <v>0</v>
@@ -7478,7 +7481,7 @@
     </row>
     <row r="20" spans="1:251" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="22" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B20" s="22">
         <f>MIN(B21:B25)</f>

</xml_diff>